<commit_message>
updated per running 13173 CDM Projects
</commit_message>
<xml_diff>
--- a/PicklistToUpdate.xlsx
+++ b/PicklistToUpdate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erickchandra/Documents/code/CADTrust/cdm-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53DA76CE-FB33-1742-947A-B99434467151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E050747E-3CAD-9348-8A84-ACF78DA7A46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="3240" windowWidth="26040" windowHeight="14760" xr2:uid="{76C61729-DDDC-BC46-8E25-00A43B528B72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Country</t>
   </si>
@@ -65,12 +65,141 @@
  'United States of America',
  'Viet Nam'}</t>
   </si>
+  <si>
+    <t>Failed to post project with ID: IYCPOCZX72JKY7I7CYXKYTG2ZU8IYO. Status code: 400. Message: {'message': 'Data Validation error', 'errors': ["projectStatus does not include a valid option Listed, Validated, Registered, Approved, Authorized, Completed, Withdrawn, De-registered instead got 'Rejected'"],</t>
+  </si>
+  <si>
+    <t>CDM Status</t>
+  </si>
+  <si>
+    <t>CAD Trust Equivalent</t>
+  </si>
+  <si>
+    <t>Registered</t>
+  </si>
+  <si>
+    <t>Withdrawn</t>
+  </si>
+  <si>
+    <t>WithdrawnBeforePublication</t>
+  </si>
+  <si>
+    <t>Withdrawn Before Publication</t>
+  </si>
+  <si>
+    <t>De-registered</t>
+  </si>
+  <si>
+    <t>Pending Publication</t>
+  </si>
+  <si>
+    <t>Provisional</t>
+  </si>
+  <si>
+    <t>Validation Replaced</t>
+  </si>
+  <si>
+    <t>Requesting Registration</t>
+  </si>
+  <si>
+    <t>Validated</t>
+  </si>
+  <si>
+    <t>Validation Public</t>
+  </si>
+  <si>
+    <t>Validation Terminated</t>
+  </si>
+  <si>
+    <t>nan (missing data)</t>
+  </si>
+  <si>
+    <t>Listed</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Not Sure About This</t>
+  </si>
+  <si>
+    <t>Authorized</t>
+  </si>
+  <si>
+    <t>ML; MR; SN</t>
+  </si>
+  <si>
+    <t>ID; MY</t>
+  </si>
+  <si>
+    <t>yemen</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Empty id bro</t>
+  </si>
+  <si>
+    <t>8459 code, 8461 real</t>
+  </si>
+  <si>
+    <t>8862 cdm got problem, 8860 code</t>
+  </si>
+  <si>
+    <t>BDF248C6JG1SKOZYQ5T3WVEHR7MXLU</t>
+  </si>
+  <si>
+    <t>9220 9218 not complete</t>
+  </si>
+  <si>
+    <t>0SERXDY1GS89I4BD3T8QL8NPI6Z34A/</t>
+  </si>
+  <si>
+    <t>9436 and 9434</t>
+  </si>
+  <si>
+    <t>A39MS6G57IZHWTBEVNPXRJOFL8K01C</t>
+  </si>
+  <si>
+    <t>9481, 9479</t>
+  </si>
+  <si>
+    <t>DB/Z31DKITEOQXOLO3V5IMYVBGQ8IYZP4</t>
+  </si>
+  <si>
+    <t>10172 and 10170</t>
+  </si>
+  <si>
+    <t>in code is 6142,8051,10220</t>
+  </si>
+  <si>
+    <t>Aux_ACG70V0UUUPNDPCRJL8KRYLHHSB0CJ</t>
+  </si>
+  <si>
+    <t>10272 and 10274</t>
+  </si>
+  <si>
+    <t>UBX0FC1NMA8IV9H5LTOEG3PJKZSWD6</t>
+  </si>
+  <si>
+    <t>D8IRSCM3W0ZGKAFXYJOQVL6HP2NEBU</t>
+  </si>
+  <si>
+    <t>11245 and 11243</t>
+  </si>
+  <si>
+    <t>EL9SWD7R6H4MKP3CB8XUYAOFN2J5TZ</t>
+  </si>
+  <si>
+    <t>11520 and 11518</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,16 +207,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,15 +268,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,20 +619,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67876A5D-857D-5D4C-8ECD-A71D75AE5857}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="62.33203125" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>8063</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34">
+        <v>10406.10404</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>